<commit_message>
Test updating excel modification
</commit_message>
<xml_diff>
--- a/PCB_BOM.xlsx
+++ b/PCB_BOM.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thedo_000\Documents\GitHubRepos\3D-Printer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18200" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
   <si>
     <t>Component</t>
   </si>
@@ -204,6 +209,9 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM319R61E106KA12D/490-5525-1-ND/2334922</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -273,6 +281,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -320,7 +331,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -355,7 +366,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -566,26 +577,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="9.140625" style="1"/>
+    <col min="10" max="10" width="34.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -617,7 +628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -649,7 +660,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -681,7 +692,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -713,7 +724,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -745,7 +756,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -777,7 +788,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -809,57 +820,84 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -884,7 +922,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -896,7 +934,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated PCB_BOM with caps
</commit_message>
<xml_diff>
--- a/PCB_BOM.xlsx
+++ b/PCB_BOM.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="77">
   <si>
     <t>Component</t>
   </si>
@@ -62,15 +62,9 @@
     <t>C8</t>
   </si>
   <si>
-    <t>C12</t>
-  </si>
-  <si>
     <t>C13</t>
   </si>
   <si>
-    <t>C14</t>
-  </si>
-  <si>
     <t>C15</t>
   </si>
   <si>
@@ -87,9 +81,6 @@
   </si>
   <si>
     <t>C20</t>
-  </si>
-  <si>
-    <t>C21</t>
   </si>
   <si>
     <t>C22</t>
@@ -202,23 +193,117 @@
     <t>GRM319R61E106KA12D</t>
   </si>
   <si>
-    <t>11 µF, 25 V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1207 (3216 Metric) </t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM319R61E106KA12D/490-5525-1-ND/2334922</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>C1206C104K5RAC7867</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 nF (0.1 µF), 50 V </t>
+  </si>
+  <si>
+    <t>1206 (3216 Metric)</t>
+  </si>
+  <si>
+    <t>Power Decoupling</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/kemet/C1206C104K5RAC7867/399-1249-1-ND/411524</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12065C103KAT2A
+</t>
+  </si>
+  <si>
+    <t>10 nF (10000 pF), 50 V</t>
+  </si>
+  <si>
+    <t>Endstop Decoupling</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/avx-corporation/12065C103KAT2A/478-1542-1-ND/564574</t>
+  </si>
+  <si>
+    <t>12065C103KAT2A</t>
+  </si>
+  <si>
+    <t>CL31B104KACNNNC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 nF (0.1 µF), 25 V </t>
+  </si>
+  <si>
+    <t>EEPROM Decoupling</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/CL31B104KACNNNC/1276-2742-1-ND/3890828</t>
+  </si>
+  <si>
+    <t>C23</t>
+  </si>
+  <si>
+    <t>C24</t>
+  </si>
+  <si>
+    <t>C25</t>
+  </si>
+  <si>
+    <t>C26</t>
+  </si>
+  <si>
+    <t>C27</t>
+  </si>
+  <si>
+    <t>C28</t>
+  </si>
+  <si>
+    <t>C1206C475Z4VACTU</t>
+  </si>
+  <si>
+    <t>4.7 µF, 16 V</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/kemet/C1206C475Z4VACTU/399-1262-1-ND/411537</t>
+  </si>
+  <si>
+    <t>UMK316BJ475KL-T</t>
+  </si>
+  <si>
+    <t>4.7 µF, 50 V</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/taiyo-yuden/UMK316BJ475KL-T/587-1962-1-ND/1646625</t>
+  </si>
+  <si>
+    <t>UWT1E221MNL1GS</t>
+  </si>
+  <si>
+    <t>220 µF, 25 V</t>
+  </si>
+  <si>
+    <t>Thermistor Circuit</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/nichicon/UWT1E221MNL1GS/493-2192-1-ND/590167</t>
+  </si>
+  <si>
+    <t>CL31F106ZOHNNNE</t>
+  </si>
+  <si>
+    <t>10 µF, 16 V</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/CL31F106ZOHNNNE/1276-1312-1-ND/3889398</t>
+  </si>
+  <si>
+    <t>CAPS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +321,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -262,12 +355,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -575,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -592,7 +691,7 @@
     <col min="7" max="7" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.08984375" style="1" customWidth="1"/>
     <col min="11" max="13" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
@@ -601,7 +700,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -619,62 +718,44 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0.1074</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0.1074</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>32</v>
-      </c>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -686,27 +767,27 @@
         <v>0.1074</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
@@ -718,27 +799,27 @@
         <v>0.1074</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
@@ -750,59 +831,59 @@
         <v>0.1074</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="F6" s="1">
         <v>1</v>
       </c>
       <c r="G6" s="1">
-        <v>0.24</v>
+        <v>0.1074</v>
       </c>
       <c r="H6" s="1">
-        <v>0.24</v>
+        <v>0.1074</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -814,105 +895,619 @@
         <v>0.24</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="10" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="D21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+    </row>
+    <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:J2"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2" display="http://www.digikey.com/product-detail/en/nichicon/UWT1H470MCL1GS/493-2225-2-ND/589966"/>
-    <hyperlink ref="J4" r:id="rId3" display="http://www.digikey.com/product-detail/en/nichicon/UWT1H470MCL1GS/493-2225-2-ND/589966"/>
-    <hyperlink ref="J5" r:id="rId4" display="http://www.digikey.com/product-detail/en/nichicon/UWT1H470MCL1GS/493-2225-2-ND/589966"/>
-    <hyperlink ref="J6" r:id="rId5"/>
-    <hyperlink ref="J7" r:id="rId6" display="http://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM319R61E106KA12D/490-5525-1-ND/2334921"/>
+    <hyperlink ref="J3" r:id="rId1"/>
+    <hyperlink ref="J4" r:id="rId2" display="http://www.digikey.com/product-detail/en/nichicon/UWT1H470MCL1GS/493-2225-2-ND/589966"/>
+    <hyperlink ref="J5" r:id="rId3" display="http://www.digikey.com/product-detail/en/nichicon/UWT1H470MCL1GS/493-2225-2-ND/589966"/>
+    <hyperlink ref="J6" r:id="rId4" display="http://www.digikey.com/product-detail/en/nichicon/UWT1H470MCL1GS/493-2225-2-ND/589966"/>
+    <hyperlink ref="J7" r:id="rId5"/>
+    <hyperlink ref="J8" r:id="rId6" display="http://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM319R61E106KA12D/490-5525-1-ND/2334921"/>
+    <hyperlink ref="J9" r:id="rId7"/>
+    <hyperlink ref="J10" r:id="rId8"/>
+    <hyperlink ref="J11" r:id="rId9"/>
+    <hyperlink ref="J12" r:id="rId10"/>
+    <hyperlink ref="J13" r:id="rId11"/>
+    <hyperlink ref="J14" r:id="rId12"/>
+    <hyperlink ref="J15" r:id="rId13"/>
+    <hyperlink ref="J16" r:id="rId14"/>
+    <hyperlink ref="J17" r:id="rId15"/>
+    <hyperlink ref="J18" r:id="rId16"/>
+    <hyperlink ref="J19" r:id="rId17"/>
+    <hyperlink ref="J20" r:id="rId18"/>
+    <hyperlink ref="J21" r:id="rId19"/>
+    <hyperlink ref="J22" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added resistor header to PCB BOM
</commit_message>
<xml_diff>
--- a/PCB_BOM.xlsx
+++ b/PCB_BOM.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thedo_000\Documents\GitHubRepos\3D-Printer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18200" windowHeight="12330"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="78">
   <si>
     <t>Component</t>
   </si>
@@ -297,6 +292,9 @@
   </si>
   <si>
     <t>CAPS</t>
+  </si>
+  <si>
+    <t>RESISTORS</t>
   </si>
 </sst>
 </file>
@@ -430,7 +428,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -465,7 +463,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -674,28 +672,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="38.08984375" style="1" customWidth="1"/>
-    <col min="11" max="13" width="9.1796875" style="1"/>
+    <col min="10" max="10" width="38.140625" style="1" customWidth="1"/>
+    <col min="11" max="13" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -727,7 +725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>76</v>
       </c>
@@ -741,7 +739,7 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -773,7 +771,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -805,7 +803,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -837,7 +835,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -869,7 +867,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -901,7 +899,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -933,7 +931,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -965,7 +963,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="57.95" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -997,7 +995,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="57.95" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1029,7 +1027,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="57.95" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1061,7 +1059,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="57.95" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -1093,7 +1091,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -1125,7 +1123,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1157,7 +1155,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -1189,7 +1187,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>57</v>
       </c>
@@ -1221,7 +1219,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
@@ -1253,7 +1251,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>59</v>
       </c>
@@ -1285,7 +1283,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>60</v>
       </c>
@@ -1320,7 +1318,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="1:13" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>61</v>
       </c>
@@ -1355,7 +1353,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="1:13" s="3" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>62</v>
       </c>
@@ -1390,22 +1388,21 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1420,7 +1417,7 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1435,7 +1432,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1450,7 +1447,7 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1465,7 +1462,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
-    <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1480,9 +1477,25 @@
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
+    <row r="29" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A23:J23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J3" r:id="rId1"/>
@@ -1517,7 +1530,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1529,7 +1542,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added connectors to PCB BOM, added some other reference docs
</commit_message>
<xml_diff>
--- a/PCB_BOM.xlsx
+++ b/PCB_BOM.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thedo_000\Documents\GitHubRepos\3D-Printer\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18200" windowHeight="12330"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="DigiKey" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="226">
   <si>
     <t>Component</t>
   </si>
@@ -677,12 +672,81 @@
   <si>
     <t>http://www.digikey.com/product-search/en/discrete-semiconductor-products/transistors-fets-mosfets-single/1376381?k=IRF3708&amp;k=&amp;pkeyword=IRF3708&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
   </si>
+  <si>
+    <t>CONNECTORS</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>JP2</t>
+  </si>
+  <si>
+    <t>JP7</t>
+  </si>
+  <si>
+    <t>JP9</t>
+  </si>
+  <si>
+    <t>1735446-4</t>
+  </si>
+  <si>
+    <t>Header, Shrouded Connector</t>
+  </si>
+  <si>
+    <t>4 Pos, 2.00 mm</t>
+  </si>
+  <si>
+    <t>0.079" (2.00mm)</t>
+  </si>
+  <si>
+    <t>Stepper Motor Interface</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/1735446-4/A100098-ND/2078000</t>
+  </si>
+  <si>
+    <t>JP4</t>
+  </si>
+  <si>
+    <t>JP15</t>
+  </si>
+  <si>
+    <t>DUE</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>DUE Pin Access</t>
+  </si>
+  <si>
+    <t>PRPC040SAAN-RC</t>
+  </si>
+  <si>
+    <t>Header, Unshrouded Connector</t>
+  </si>
+  <si>
+    <t>40 pos, 2.54 mm</t>
+  </si>
+  <si>
+    <t>0.100" (2.54mm) Through Hole</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/PRPC040SAAN-RC/S1011EC-40-ND/2775214</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/PRPC040SAAN-RC/S1011EC-40-ND/2775215</t>
+  </si>
+  <si>
+    <t>End Stops</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -712,6 +776,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -734,7 +805,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -747,6 +818,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -809,7 +895,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -844,7 +930,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1053,52 +1139,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K80"/>
+  <dimension ref="A1:K94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="51" style="1" customWidth="1"/>
-    <col min="9" max="11" width="9.1796875" style="1"/>
+    <col min="9" max="11" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>174</v>
       </c>
@@ -1110,7 +1197,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>175</v>
       </c>
@@ -1136,7 +1223,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>182</v>
       </c>
@@ -1162,7 +1249,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>188</v>
       </c>
@@ -1174,7 +1261,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>189</v>
       </c>
@@ -1200,7 +1287,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>190</v>
       </c>
@@ -1226,7 +1313,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>191</v>
       </c>
@@ -1252,7 +1339,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>192</v>
       </c>
@@ -1278,7 +1365,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>193</v>
       </c>
@@ -1304,7 +1391,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>194</v>
       </c>
@@ -1330,7 +1417,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>167</v>
       </c>
@@ -1342,7 +1429,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>168</v>
       </c>
@@ -1368,7 +1455,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>74</v>
       </c>
@@ -1380,7 +1467,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -1406,7 +1493,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -1432,7 +1519,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -1458,7 +1545,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1484,7 +1571,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -1510,7 +1597,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
@@ -1536,7 +1623,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -1562,7 +1649,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -1588,7 +1675,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
@@ -1614,7 +1701,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
@@ -1640,7 +1727,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
@@ -1666,7 +1753,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
@@ -1692,7 +1779,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>18</v>
       </c>
@@ -1718,7 +1805,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
@@ -1744,7 +1831,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>55</v>
       </c>
@@ -1770,7 +1857,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>56</v>
       </c>
@@ -1796,7 +1883,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>57</v>
       </c>
@@ -1822,7 +1909,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>58</v>
       </c>
@@ -1851,7 +1938,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>59</v>
       </c>
@@ -1880,7 +1967,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>60</v>
       </c>
@@ -1909,7 +1996,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>75</v>
       </c>
@@ -1921,7 +2008,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:11" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>76</v>
       </c>
@@ -1950,7 +2037,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>77</v>
       </c>
@@ -1979,7 +2066,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>78</v>
       </c>
@@ -2008,7 +2095,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>79</v>
       </c>
@@ -2037,7 +2124,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>80</v>
       </c>
@@ -2066,7 +2153,7 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>81</v>
       </c>
@@ -2095,7 +2182,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>82</v>
       </c>
@@ -2121,7 +2208,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>83</v>
       </c>
@@ -2147,7 +2234,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>84</v>
       </c>
@@ -2173,7 +2260,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>85</v>
       </c>
@@ -2199,7 +2286,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>86</v>
       </c>
@@ -2225,7 +2312,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>87</v>
       </c>
@@ -2251,7 +2338,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>88</v>
       </c>
@@ -2277,7 +2364,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>89</v>
       </c>
@@ -2303,7 +2390,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>90</v>
       </c>
@@ -2329,7 +2416,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>91</v>
       </c>
@@ -2355,7 +2442,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>92</v>
       </c>
@@ -2381,7 +2468,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>93</v>
       </c>
@@ -2407,7 +2494,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>94</v>
       </c>
@@ -2433,7 +2520,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>95</v>
       </c>
@@ -2459,7 +2546,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>96</v>
       </c>
@@ -2485,7 +2572,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>97</v>
       </c>
@@ -2511,7 +2598,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>98</v>
       </c>
@@ -2537,7 +2624,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>99</v>
       </c>
@@ -2563,7 +2650,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>100</v>
       </c>
@@ -2589,7 +2676,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>101</v>
       </c>
@@ -2615,7 +2702,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>129</v>
       </c>
@@ -2627,7 +2714,7 @@
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
     </row>
-    <row r="63" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>130</v>
       </c>
@@ -2653,7 +2740,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>131</v>
       </c>
@@ -2679,7 +2766,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>132</v>
       </c>
@@ -2705,7 +2792,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>133</v>
       </c>
@@ -2731,7 +2818,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>134</v>
       </c>
@@ -2757,7 +2844,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>135</v>
       </c>
@@ -2783,7 +2870,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>136</v>
       </c>
@@ -2809,7 +2896,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>137</v>
       </c>
@@ -2835,7 +2922,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>138</v>
       </c>
@@ -2861,7 +2948,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>153</v>
       </c>
@@ -2873,7 +2960,7 @@
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
     </row>
-    <row r="73" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>154</v>
       </c>
@@ -2899,7 +2986,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>155</v>
       </c>
@@ -2925,7 +3012,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>156</v>
       </c>
@@ -2951,7 +3038,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>157</v>
       </c>
@@ -2977,7 +3064,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>158</v>
       </c>
@@ -3003,7 +3090,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>159</v>
       </c>
@@ -3029,7 +3116,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>160</v>
       </c>
@@ -3055,7 +3142,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>161</v>
       </c>
@@ -3081,15 +3168,279 @@
         <v>166</v>
       </c>
     </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="4"/>
+      <c r="H81" s="4"/>
+    </row>
+    <row r="82" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F82" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F83" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F84" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F85" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F86" s="6">
+        <v>0.74</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H86" s="7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H87" s="6"/>
+    </row>
+    <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B88" s="6"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H88" s="6"/>
+    </row>
+    <row r="89" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F89" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F90" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
+      <c r="D91" s="8"/>
+      <c r="E91" s="8"/>
+      <c r="F91" s="8"/>
+      <c r="G91" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H91" s="8"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B92" s="8"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="8"/>
+      <c r="F92" s="8"/>
+      <c r="H92" s="9"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B93" s="8"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="8"/>
+      <c r="H93" s="8"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B94" s="8"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
+      <c r="E94" s="8"/>
+      <c r="F94" s="8"/>
+      <c r="H94" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="14">
+    <mergeCell ref="A72:H72"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A81:H81"/>
+    <mergeCell ref="B86:B88"/>
+    <mergeCell ref="C86:C88"/>
+    <mergeCell ref="D86:D88"/>
+    <mergeCell ref="E86:E88"/>
+    <mergeCell ref="F86:F88"/>
+    <mergeCell ref="H86:H88"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="A35:H35"/>
     <mergeCell ref="A62:H62"/>
-    <mergeCell ref="A72:H72"/>
-    <mergeCell ref="A12:H12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H15" r:id="rId1"/>
@@ -3164,9 +3515,16 @@
     <hyperlink ref="H9" r:id="rId70"/>
     <hyperlink ref="H10" r:id="rId71"/>
     <hyperlink ref="H11" r:id="rId72"/>
+    <hyperlink ref="H82" r:id="rId73"/>
+    <hyperlink ref="H83" r:id="rId74"/>
+    <hyperlink ref="H84" r:id="rId75"/>
+    <hyperlink ref="H85" r:id="rId76"/>
+    <hyperlink ref="H86" r:id="rId77"/>
+    <hyperlink ref="H89" r:id="rId78" display="http://www.digikey.com/product-detail/en/sullins-connector-solutions/PRPC040SAAN-RC/S1011EC-40-ND/2775214"/>
+    <hyperlink ref="H90" r:id="rId79" display="http://www.digikey.com/product-detail/en/sullins-connector-solutions/PRPC040SAAN-RC/S1011EC-40-ND/2775214"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId73"/>
+  <pageSetup orientation="portrait" r:id="rId80"/>
 </worksheet>
 </file>
 
@@ -3176,7 +3534,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3188,7 +3546,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished first rev of PCB BOM and started eagle schematic
</commit_message>
<xml_diff>
--- a/PCB_BOM.xlsx
+++ b/PCB_BOM.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thedo_000\Documents\GitHubRepos\3D-Printer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18200" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="DigiKey" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="244">
   <si>
     <t>Component</t>
   </si>
@@ -740,6 +745,60 @@
   </si>
   <si>
     <t>End Stops</t>
+  </si>
+  <si>
+    <t>Xmin</t>
+  </si>
+  <si>
+    <t>Xmax</t>
+  </si>
+  <si>
+    <t>Ymin</t>
+  </si>
+  <si>
+    <t>Ymax</t>
+  </si>
+  <si>
+    <t>Zmin</t>
+  </si>
+  <si>
+    <t>Zmax</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>MJTP1230</t>
+  </si>
+  <si>
+    <t>Tactile Switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SPST-NO Top Actuated Through Hole</t>
+  </si>
+  <si>
+    <t>6.00mm x 6.00mm, Through Hole</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/apem-inc/MJTP1230/679-2428-ND/1798037</t>
+  </si>
+  <si>
+    <t>Stepper Controller IO</t>
+  </si>
+  <si>
+    <t>PPTC081LFBN-RC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female Header </t>
+  </si>
+  <si>
+    <t>8 Pos, 2.54 mm</t>
+  </si>
+  <si>
+    <t>Interface DRV8825 Modules</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/sullins-connector-solutions/PPTC081LFBN-RC/S7006-ND/810147</t>
   </si>
 </sst>
 </file>
@@ -784,12 +843,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -805,7 +870,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -816,9 +881,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -828,11 +890,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -895,7 +966,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -930,7 +1001,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1139,65 +1210,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K94"/>
+  <dimension ref="A1:K106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G91" sqref="G91"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="51" style="1" customWidth="1"/>
-    <col min="9" max="11" width="9.140625" style="1"/>
+    <col min="9" max="11" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>175</v>
       </c>
@@ -1223,7 +1294,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>182</v>
       </c>
@@ -1249,45 +1320,45 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="10">
         <v>1.78</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="11" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>190</v>
       </c>
@@ -1313,7 +1384,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>191</v>
       </c>
@@ -1339,7 +1410,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>192</v>
       </c>
@@ -1365,7 +1436,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>193</v>
       </c>
@@ -1391,7 +1462,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>194</v>
       </c>
@@ -1417,19 +1488,19 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>168</v>
       </c>
@@ -1455,19 +1526,19 @@
         <v>173</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -1493,7 +1564,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
@@ -1519,7 +1590,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -1545,7 +1616,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1571,7 +1642,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -1597,7 +1668,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
@@ -1623,7 +1694,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -1649,7 +1720,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -1675,7 +1746,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
@@ -1701,7 +1772,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
@@ -1727,7 +1798,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
@@ -1753,7 +1824,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
@@ -1779,7 +1850,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>18</v>
       </c>
@@ -1805,7 +1876,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
@@ -1831,7 +1902,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>55</v>
       </c>
@@ -1857,7 +1928,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>56</v>
       </c>
@@ -1883,7 +1954,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>57</v>
       </c>
@@ -1909,7 +1980,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>58</v>
       </c>
@@ -1938,7 +2009,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>59</v>
       </c>
@@ -1967,7 +2038,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>60</v>
       </c>
@@ -1996,19 +2067,19 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A35" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+    </row>
+    <row r="36" spans="1:11" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>76</v>
       </c>
@@ -2037,7 +2108,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>77</v>
       </c>
@@ -2066,7 +2137,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>78</v>
       </c>
@@ -2095,7 +2166,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>79</v>
       </c>
@@ -2124,7 +2195,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>80</v>
       </c>
@@ -2153,7 +2224,7 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>81</v>
       </c>
@@ -2182,7 +2253,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>82</v>
       </c>
@@ -2208,7 +2279,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>83</v>
       </c>
@@ -2234,7 +2305,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>84</v>
       </c>
@@ -2260,7 +2331,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>85</v>
       </c>
@@ -2286,7 +2357,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>86</v>
       </c>
@@ -2312,7 +2383,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>87</v>
       </c>
@@ -2338,7 +2409,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>88</v>
       </c>
@@ -2364,7 +2435,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>89</v>
       </c>
@@ -2390,7 +2461,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>90</v>
       </c>
@@ -2416,7 +2487,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>91</v>
       </c>
@@ -2442,7 +2513,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>92</v>
       </c>
@@ -2468,7 +2539,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>93</v>
       </c>
@@ -2494,7 +2565,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>94</v>
       </c>
@@ -2520,7 +2591,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>95</v>
       </c>
@@ -2546,7 +2617,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>96</v>
       </c>
@@ -2572,7 +2643,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>97</v>
       </c>
@@ -2598,7 +2669,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>98</v>
       </c>
@@ -2624,7 +2695,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>99</v>
       </c>
@@ -2650,7 +2721,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>100</v>
       </c>
@@ -2676,7 +2747,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>101</v>
       </c>
@@ -2702,19 +2773,19 @@
         <v>128</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-    </row>
-    <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+    </row>
+    <row r="63" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>130</v>
       </c>
@@ -2740,7 +2811,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>131</v>
       </c>
@@ -2766,7 +2837,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>132</v>
       </c>
@@ -2792,7 +2863,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>133</v>
       </c>
@@ -2818,7 +2889,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>134</v>
       </c>
@@ -2844,7 +2915,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>135</v>
       </c>
@@ -2870,7 +2941,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>136</v>
       </c>
@@ -2896,7 +2967,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>137</v>
       </c>
@@ -2922,7 +2993,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>138</v>
       </c>
@@ -2948,19 +3019,19 @@
         <v>143</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A72" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
-    </row>
-    <row r="73" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+    </row>
+    <row r="73" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>154</v>
       </c>
@@ -2986,7 +3057,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>155</v>
       </c>
@@ -3012,7 +3083,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>156</v>
       </c>
@@ -3038,7 +3109,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>157</v>
       </c>
@@ -3064,7 +3135,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>158</v>
       </c>
@@ -3090,7 +3161,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>159</v>
       </c>
@@ -3116,7 +3187,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>160</v>
       </c>
@@ -3142,7 +3213,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>161</v>
       </c>
@@ -3168,19 +3239,19 @@
         <v>166</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A81" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="4"/>
-      <c r="G81" s="4"/>
-      <c r="H81" s="4"/>
-    </row>
-    <row r="82" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
+    </row>
+    <row r="82" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>204</v>
       </c>
@@ -3206,7 +3277,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>205</v>
       </c>
@@ -3232,7 +3303,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>206</v>
       </c>
@@ -3258,7 +3329,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>207</v>
       </c>
@@ -3284,61 +3355,61 @@
         <v>213</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B86" s="6" t="s">
+      <c r="B86" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C86" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="D86" s="6" t="s">
+      <c r="D86" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="E86" s="6" t="s">
+      <c r="E86" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="F86" s="6">
+      <c r="F86" s="8">
         <v>0.74</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H86" s="7" t="s">
+      <c r="H86" s="9" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="B87" s="6"/>
-      <c r="C87" s="6"/>
-      <c r="D87" s="6"/>
-      <c r="E87" s="6"/>
-      <c r="F87" s="6"/>
+      <c r="B87" s="8"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="8"/>
+      <c r="E87" s="8"/>
+      <c r="F87" s="8"/>
       <c r="G87" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="H87" s="6"/>
-    </row>
-    <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H87" s="8"/>
+    </row>
+    <row r="88" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B88" s="6"/>
-      <c r="C88" s="6"/>
-      <c r="D88" s="6"/>
-      <c r="E88" s="6"/>
-      <c r="F88" s="6"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="8"/>
       <c r="G88" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="H88" s="6"/>
-    </row>
-    <row r="89" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="H88" s="8"/>
+    </row>
+    <row r="89" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>216</v>
       </c>
@@ -3364,7 +3435,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>216</v>
       </c>
@@ -3386,47 +3457,384 @@
       <c r="G90" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="H90" s="2" t="s">
+      <c r="H90" s="6" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B91" s="8"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
-      <c r="F91" s="8"/>
-      <c r="G91" s="1" t="s">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="D91" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="E91" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="F91" s="8">
+        <v>0.74</v>
+      </c>
+      <c r="G91" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="H91" s="8"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H91" s="9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
+        <v>227</v>
+      </c>
       <c r="B92" s="8"/>
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
       <c r="E92" s="8"/>
       <c r="F92" s="8"/>
-      <c r="H92" s="9"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G92" s="8"/>
+      <c r="H92" s="8"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
       <c r="D93" s="8"/>
       <c r="E93" s="8"/>
       <c r="F93" s="8"/>
+      <c r="G93" s="8"/>
       <c r="H93" s="8"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
+        <v>229</v>
+      </c>
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
       <c r="D94" s="8"/>
       <c r="E94" s="8"/>
       <c r="F94" s="8"/>
+      <c r="G94" s="8"/>
       <c r="H94" s="8"/>
     </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B95" s="8"/>
+      <c r="C95" s="8"/>
+      <c r="D95" s="8"/>
+      <c r="E95" s="8"/>
+      <c r="F95" s="8"/>
+      <c r="G95" s="8"/>
+      <c r="H95" s="8"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B96" s="8"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="8"/>
+      <c r="E96" s="8"/>
+      <c r="F96" s="8"/>
+      <c r="G96" s="8"/>
+      <c r="H96" s="8"/>
+    </row>
+    <row r="97" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A97" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F97" s="5">
+        <v>0.86</v>
+      </c>
+      <c r="G97" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="H97" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="I97" s="5"/>
+      <c r="J97" s="5"/>
+      <c r="K97" s="5"/>
+    </row>
+    <row r="98" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A98" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F98" s="5">
+        <v>0.86</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="H98" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="I98" s="5"/>
+      <c r="J98" s="5"/>
+      <c r="K98" s="5"/>
+    </row>
+    <row r="99" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A99" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F99" s="5">
+        <v>0.86</v>
+      </c>
+      <c r="G99" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="H99" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="I99" s="5"/>
+      <c r="J99" s="5"/>
+      <c r="K99" s="5"/>
+    </row>
+    <row r="100" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A100" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F100" s="5">
+        <v>0.86</v>
+      </c>
+      <c r="G100" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="H100" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="I100" s="5"/>
+      <c r="J100" s="5"/>
+      <c r="K100" s="5"/>
+    </row>
+    <row r="101" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A101" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F101" s="5">
+        <v>0.86</v>
+      </c>
+      <c r="G101" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="H101" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="I101" s="5"/>
+      <c r="J101" s="5"/>
+      <c r="K101" s="5"/>
+    </row>
+    <row r="102" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A102" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F102" s="5">
+        <v>0.86</v>
+      </c>
+      <c r="G102" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="H102" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="I102" s="5"/>
+      <c r="J102" s="5"/>
+      <c r="K102" s="5"/>
+    </row>
+    <row r="103" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A103" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F103" s="5">
+        <v>0.86</v>
+      </c>
+      <c r="G103" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="H103" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="I103" s="5"/>
+      <c r="J103" s="5"/>
+      <c r="K103" s="5"/>
+    </row>
+    <row r="104" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A104" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F104" s="5">
+        <v>0.86</v>
+      </c>
+      <c r="G104" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="H104" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="I104" s="5"/>
+      <c r="J104" s="5"/>
+      <c r="K104" s="5"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A105" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B105" s="7"/>
+      <c r="C105" s="7"/>
+      <c r="D105" s="7"/>
+      <c r="E105" s="7"/>
+      <c r="F105" s="7"/>
+      <c r="G105" s="7"/>
+      <c r="H105" s="7"/>
+      <c r="I105" s="5"/>
+      <c r="J105" s="5"/>
+      <c r="K105" s="5"/>
+    </row>
+    <row r="106" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A106" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F106" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H106" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="22">
+    <mergeCell ref="G91:G96"/>
+    <mergeCell ref="H91:H96"/>
+    <mergeCell ref="A105:H105"/>
+    <mergeCell ref="B91:B96"/>
+    <mergeCell ref="C91:C96"/>
+    <mergeCell ref="D91:D96"/>
+    <mergeCell ref="E91:E96"/>
+    <mergeCell ref="F91:F96"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A62:H62"/>
     <mergeCell ref="A72:H72"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="A81:H81"/>
@@ -3436,11 +3844,6 @@
     <mergeCell ref="E86:E88"/>
     <mergeCell ref="F86:F88"/>
     <mergeCell ref="H86:H88"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="A62:H62"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H15" r:id="rId1"/>
@@ -3521,10 +3924,20 @@
     <hyperlink ref="H85" r:id="rId76"/>
     <hyperlink ref="H86" r:id="rId77"/>
     <hyperlink ref="H89" r:id="rId78" display="http://www.digikey.com/product-detail/en/sullins-connector-solutions/PRPC040SAAN-RC/S1011EC-40-ND/2775214"/>
-    <hyperlink ref="H90" r:id="rId79" display="http://www.digikey.com/product-detail/en/sullins-connector-solutions/PRPC040SAAN-RC/S1011EC-40-ND/2775214"/>
+    <hyperlink ref="H90" r:id="rId79"/>
+    <hyperlink ref="H91" r:id="rId80"/>
+    <hyperlink ref="H106" r:id="rId81"/>
+    <hyperlink ref="H97" r:id="rId82"/>
+    <hyperlink ref="H98" r:id="rId83"/>
+    <hyperlink ref="H99" r:id="rId84"/>
+    <hyperlink ref="H100" r:id="rId85"/>
+    <hyperlink ref="H101" r:id="rId86"/>
+    <hyperlink ref="H102" r:id="rId87"/>
+    <hyperlink ref="H103" r:id="rId88"/>
+    <hyperlink ref="H104" r:id="rId89"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId80"/>
+  <pageSetup orientation="portrait" r:id="rId90"/>
 </worksheet>
 </file>
 
@@ -3534,7 +3947,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3546,7 +3959,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>